<commit_message>
Aanpassingen obv feedback CdH
</commit_message>
<xml_diff>
--- a/R/data/dfPersona_per_group.xlsx
+++ b/R/data/dfPersona_per_group.xlsx
@@ -390,12 +390,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Aansluiting</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Vooropleiding</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Aansluiting</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -541,12 +541,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Direct</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>HAVO</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Direct</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -661,12 +661,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>Direct</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>HAVO</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Direct</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -757,22 +757,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Vooropleiding</t>
+          <t>Aansluiting</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BD</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="C4">
         <v>1613</v>
       </c>
       <c r="D4">
-        <v>92</v>
+        <v>756</v>
       </c>
       <c r="E4">
-        <v>0.057</v>
+        <v>0.469</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -781,22 +781,22 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>BD</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>HAVO</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Onbekend</t>
+          <t>MedV</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Onbekend</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -835,13 +835,13 @@
         </is>
       </c>
       <c r="R4">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="S4">
-        <v>126</v>
+        <v>137.5</v>
       </c>
       <c r="T4">
-        <v>15.5</v>
+        <v>34.2</v>
       </c>
       <c r="U4">
         <v>6.4</v>
@@ -862,7 +862,7 @@
         <v>6.2</v>
       </c>
       <c r="AA4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AB4">
         <v>0</v>
@@ -871,47 +871,47 @@
         <v>0</v>
       </c>
       <c r="AD4">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Vooropleiding</t>
+          <t>Aansluiting</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>Tussenjaar</t>
         </is>
       </c>
       <c r="C5">
         <v>1613</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>176</v>
       </c>
       <c r="E5">
-        <v>0.019</v>
+        <v>0.109</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>Tussenjaar</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Na CD</t>
+          <t>HAVO</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Onbekend</t>
+          <t>MedV</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -955,13 +955,13 @@
         </is>
       </c>
       <c r="R5">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S5">
-        <v>127.5</v>
+        <v>134.5</v>
       </c>
       <c r="T5">
-        <v>29.6</v>
+        <v>34.7</v>
       </c>
       <c r="U5">
         <v>6.4</v>
@@ -982,37 +982,37 @@
         <v>6.2</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AB5">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC5">
         <v>0</v>
       </c>
       <c r="AD5">
-        <v>2017.5</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Vooropleiding</t>
+          <t>Aansluiting</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>HAVO</t>
+          <t>Switch intern</t>
         </is>
       </c>
       <c r="C6">
         <v>1613</v>
       </c>
       <c r="D6">
-        <v>860</v>
+        <v>202</v>
       </c>
       <c r="E6">
-        <v>0.533</v>
+        <v>0.125</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -1021,14 +1021,14 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>Switch intern</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>HAVO</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Direct</t>
-        </is>
-      </c>
       <c r="I6" t="inlineStr">
         <is>
           <t>EM&amp;CM</t>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -1075,13 +1075,13 @@
         </is>
       </c>
       <c r="R6">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="S6">
-        <v>132</v>
+        <v>128.5</v>
       </c>
       <c r="T6">
-        <v>35.9</v>
+        <v>28.1</v>
       </c>
       <c r="U6">
         <v>6.4</v>
@@ -1102,7 +1102,7 @@
         <v>6.2</v>
       </c>
       <c r="AA6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <v>0</v>
@@ -1111,47 +1111,47 @@
         <v>0</v>
       </c>
       <c r="AD6">
-        <v>2016</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Vooropleiding</t>
+          <t>Aansluiting</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>HO</t>
+          <t>Switch extern</t>
         </is>
       </c>
       <c r="C7">
         <v>1613</v>
       </c>
       <c r="D7">
-        <v>51</v>
+        <v>445</v>
       </c>
       <c r="E7">
-        <v>0.032</v>
+        <v>0.276</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>HO</t>
+          <t>Switch extern</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Switch extern</t>
+          <t>HAVO</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Onbekend</t>
+          <t>EM</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1198,10 +1198,10 @@
         <v>20</v>
       </c>
       <c r="S7">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="T7">
-        <v>38.3</v>
+        <v>36.1</v>
       </c>
       <c r="U7">
         <v>6.4</v>
@@ -1222,10 +1222,10 @@
         <v>6.2</v>
       </c>
       <c r="AA7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AB7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -1237,22 +1237,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Vooropleiding</t>
+          <t>Aansluiting</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MBO</t>
+          <t>2e Studie</t>
         </is>
       </c>
       <c r="C8">
         <v>1613</v>
       </c>
       <c r="D8">
-        <v>522</v>
+        <v>15</v>
       </c>
       <c r="E8">
-        <v>0.324</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1261,17 +1261,17 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>MBO</t>
+          <t>2e Studie</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>HAVO</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>MedV</t>
+          <t>EM</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1315,13 +1315,13 @@
         </is>
       </c>
       <c r="R8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S8">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="T8">
-        <v>32.7</v>
+        <v>29.8</v>
       </c>
       <c r="U8">
         <v>6.4</v>
@@ -1345,34 +1345,34 @@
         <v>0</v>
       </c>
       <c r="AB8">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC8">
         <v>0</v>
       </c>
       <c r="AD8">
-        <v>2017</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Vooropleiding</t>
+          <t>Aansluiting</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>VWO</t>
+          <t>Na CD</t>
         </is>
       </c>
       <c r="C9">
         <v>1613</v>
       </c>
       <c r="D9">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="E9">
-        <v>0.036</v>
+        <v>0.012</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1381,17 +1381,17 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>VWO</t>
+          <t>Na CD</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Switch extern</t>
+          <t>CD</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>EM</t>
+          <t>EM&amp;CM</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1401,27 +1401,27 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1435,13 +1435,13 @@
         </is>
       </c>
       <c r="R9">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="S9">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="T9">
-        <v>30.9</v>
+        <v>30.5</v>
       </c>
       <c r="U9">
         <v>6.4</v>
@@ -1462,7 +1462,7 @@
         <v>6.2</v>
       </c>
       <c r="AA9">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AB9">
         <v>0</v>
@@ -1471,28 +1471,28 @@
         <v>0</v>
       </c>
       <c r="AD9">
-        <v>2016</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Aansluiting</t>
+          <t>Vooropleiding</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2e Studie</t>
+          <t>MBO</t>
         </is>
       </c>
       <c r="C10">
         <v>1613</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>522</v>
       </c>
       <c r="E10">
-        <v>0.008999999999999999</v>
+        <v>0.324</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1501,17 +1501,17 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>HAVO</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2e Studie</t>
+          <t>MBO</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Onbekend</t>
+          <t>MedV</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1555,13 +1555,13 @@
         </is>
       </c>
       <c r="R10">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S10">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="T10">
-        <v>29.8</v>
+        <v>32.7</v>
       </c>
       <c r="U10">
         <v>6.4</v>
@@ -1585,34 +1585,34 @@
         <v>0</v>
       </c>
       <c r="AB10">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC10">
         <v>0</v>
       </c>
       <c r="AD10">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Aansluiting</t>
+          <t>Vooropleiding</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>HAVO</t>
         </is>
       </c>
       <c r="C11">
         <v>1613</v>
       </c>
       <c r="D11">
-        <v>756</v>
+        <v>860</v>
       </c>
       <c r="E11">
-        <v>0.469</v>
+        <v>0.533</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1621,17 +1621,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
+          <t>Direct</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
           <t>HAVO</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Direct</t>
-        </is>
-      </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>MedV</t>
+          <t>EM&amp;CM</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1641,27 +1641,27 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1678,10 +1678,10 @@
         <v>19</v>
       </c>
       <c r="S11">
-        <v>137.5</v>
+        <v>132</v>
       </c>
       <c r="T11">
-        <v>34.2</v>
+        <v>35.9</v>
       </c>
       <c r="U11">
         <v>6.4</v>
@@ -1717,91 +1717,91 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Aansluiting</t>
+          <t>Vooropleiding</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Na CD</t>
+          <t>VWO</t>
         </is>
       </c>
       <c r="C12">
         <v>1613</v>
       </c>
       <c r="D12">
+        <v>58</v>
+      </c>
+      <c r="E12">
+        <v>0.036</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Switch extern</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>VWO</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>EM</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="R12">
         <v>19</v>
       </c>
-      <c r="E12">
-        <v>0.012</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Na CD</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Onbekend</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="R12">
-        <v>22</v>
-      </c>
       <c r="S12">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="T12">
-        <v>30.5</v>
+        <v>30.9</v>
       </c>
       <c r="U12">
         <v>6.4</v>
@@ -1822,7 +1822,7 @@
         <v>6.2</v>
       </c>
       <c r="AA12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AB12">
         <v>0</v>
@@ -1831,28 +1831,28 @@
         <v>0</v>
       </c>
       <c r="AD12">
-        <v>2012</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Aansluiting</t>
+          <t>Vooropleiding</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Switch extern</t>
+          <t>BD</t>
         </is>
       </c>
       <c r="C13">
         <v>1613</v>
       </c>
       <c r="D13">
-        <v>445</v>
+        <v>92</v>
       </c>
       <c r="E13">
-        <v>0.276</v>
+        <v>0.057</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1861,47 +1861,47 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>HAVO</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Switch extern</t>
+          <t>BD</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
+          <t>EM</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
           <t>Onbekend</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1915,13 +1915,13 @@
         </is>
       </c>
       <c r="R13">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S13">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="T13">
-        <v>36.1</v>
+        <v>15.5</v>
       </c>
       <c r="U13">
         <v>6.4</v>
@@ -1951,28 +1951,28 @@
         <v>0</v>
       </c>
       <c r="AD13">
-        <v>2015</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Aansluiting</t>
+          <t>Vooropleiding</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Switch intern</t>
+          <t>CD</t>
         </is>
       </c>
       <c r="C14">
         <v>1613</v>
       </c>
       <c r="D14">
-        <v>202</v>
+        <v>30</v>
       </c>
       <c r="E14">
-        <v>0.125</v>
+        <v>0.019</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1981,17 +1981,17 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>HAVO</t>
+          <t>Na CD</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Switch intern</t>
+          <t>CD</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Onbekend</t>
+          <t>EM</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -2001,22 +2001,22 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
@@ -2035,13 +2035,13 @@
         </is>
       </c>
       <c r="R14">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S14">
-        <v>128.5</v>
+        <v>127.5</v>
       </c>
       <c r="T14">
-        <v>28.1</v>
+        <v>29.6</v>
       </c>
       <c r="U14">
         <v>6.4</v>
@@ -2065,34 +2065,34 @@
         <v>0</v>
       </c>
       <c r="AB14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC14">
         <v>0</v>
       </c>
       <c r="AD14">
-        <v>2018</v>
+        <v>2017.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Aansluiting</t>
+          <t>Vooropleiding</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Tussenjaar</t>
+          <t>HO</t>
         </is>
       </c>
       <c r="C15">
         <v>1613</v>
       </c>
       <c r="D15">
-        <v>176</v>
+        <v>51</v>
       </c>
       <c r="E15">
-        <v>0.109</v>
+        <v>0.032</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -2101,17 +2101,17 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>HAVO</t>
+          <t>Switch extern</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Tussenjaar</t>
+          <t>HO</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>MedV</t>
+          <t>EM</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2121,27 +2121,27 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -2158,10 +2158,10 @@
         <v>20</v>
       </c>
       <c r="S15">
-        <v>134.5</v>
+        <v>128</v>
       </c>
       <c r="T15">
-        <v>34.7</v>
+        <v>38.3</v>
       </c>
       <c r="U15">
         <v>6.4</v>
@@ -2185,13 +2185,13 @@
         <v>0.1</v>
       </c>
       <c r="AB15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AC15">
         <v>0</v>
       </c>
       <c r="AD15">
-        <v>2017</v>
+        <v>2015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>